<commit_message>
Add new problems to Excel, update old values
</commit_message>
<xml_diff>
--- a/excel/Tracking.xlsx
+++ b/excel/Tracking.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="1-7" sheetId="1" r:id="rId1"/>
+    <sheet name="8-14" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="18">
   <si>
     <t xml:space="preserve"> Chapter </t>
   </si>
@@ -64,13 +65,28 @@
   <si>
     <t>Distribution of Problems</t>
   </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>% Done</t>
+  </si>
+  <si>
+    <t>% Remaining</t>
+  </si>
+  <si>
+    <t>Distributions per Type</t>
+  </si>
+  <si>
+    <t>Distribution over all</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -109,7 +125,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -122,8 +138,20 @@
         <bgColor theme="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor theme="9" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor theme="9" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -166,12 +194,65 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -180,10 +261,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -201,12 +279,171 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="36">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.0%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.0%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.0%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.0%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.0%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.0%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -226,120 +463,6 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="168" formatCode="0.0%"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="168" formatCode="0.0%"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="168" formatCode="0.0%"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="168" formatCode="0.0%"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="168" formatCode="0.0%"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="168" formatCode="0.0%"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -595,7 +718,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$R$7:$R$14</c:f>
+              <c:f>'1-7'!$R$7:$R$14</c:f>
               <c:strCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
@@ -627,7 +750,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$S$7:$S$14</c:f>
+              <c:f>'1-7'!$S$7:$S$14</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="8"/>
@@ -647,13 +770,13 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.7344632768361582</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -670,11 +793,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="385895504"/>
-        <c:axId val="430796216"/>
+        <c:axId val="503721080"/>
+        <c:axId val="503720688"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="385895504"/>
+        <c:axId val="503721080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -748,7 +871,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="430796216"/>
+        <c:crossAx val="503720688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -756,7 +879,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="430796216"/>
+        <c:axId val="503720688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -838,7 +961,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="385895504"/>
+        <c:crossAx val="503721080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1043,7 +1166,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$R$7:$R$14</c:f>
+              <c:f>'1-7'!$R$7:$R$14</c:f>
               <c:strCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
@@ -1075,7 +1198,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$T$7:$T$14</c:f>
+              <c:f>'1-7'!$T$7:$T$14</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1092,16 +1215,16 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.42372881355932202</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.59692307692307689</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1118,11 +1241,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="507789192"/>
-        <c:axId val="507793112"/>
+        <c:axId val="494466096"/>
+        <c:axId val="494467272"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="507789192"/>
+        <c:axId val="494466096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1196,7 +1319,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="507793112"/>
+        <c:crossAx val="494467272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1204,7 +1327,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="507793112"/>
+        <c:axId val="494467272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1286,7 +1409,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="507789192"/>
+        <c:crossAx val="494466096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2489,16 +2612,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B18:H26" totalsRowShown="0" headerRowDxfId="27" dataDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B18:H26" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
   <autoFilter ref="B18:H26"/>
   <tableColumns count="7">
-    <tableColumn id="1" name=" Chapter " dataDxfId="35"/>
-    <tableColumn id="2" name=" Discussion " dataDxfId="34"/>
-    <tableColumn id="3" name=" Exercises " dataDxfId="33"/>
-    <tableColumn id="4" name=" Problems " dataDxfId="32"/>
-    <tableColumn id="5" name=" Challenge " dataDxfId="31"/>
-    <tableColumn id="6" name=" Passage " dataDxfId="30"/>
-    <tableColumn id="7" name=" Total " dataDxfId="29">
+    <tableColumn id="1" name=" Chapter " dataDxfId="33"/>
+    <tableColumn id="2" name=" Discussion " dataDxfId="32"/>
+    <tableColumn id="3" name=" Exercises " dataDxfId="31"/>
+    <tableColumn id="4" name=" Problems " dataDxfId="30"/>
+    <tableColumn id="5" name=" Challenge " dataDxfId="29"/>
+    <tableColumn id="6" name=" Passage " dataDxfId="28"/>
+    <tableColumn id="7" name=" Total " dataDxfId="27">
       <calculatedColumnFormula>SUM(B19:G19)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2507,16 +2630,16 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B6:H14" totalsRowShown="0" headerRowDxfId="18" dataDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B6:H14" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
   <autoFilter ref="B6:H14"/>
   <tableColumns count="7">
-    <tableColumn id="1" name=" Chapter " dataDxfId="26"/>
-    <tableColumn id="2" name=" Discussion " dataDxfId="25"/>
-    <tableColumn id="3" name=" Exercises " dataDxfId="24"/>
-    <tableColumn id="4" name=" Problems " dataDxfId="23"/>
-    <tableColumn id="5" name=" Challenge " dataDxfId="22"/>
-    <tableColumn id="6" name=" Passage " dataDxfId="21"/>
-    <tableColumn id="7" name=" Total " dataDxfId="20">
+    <tableColumn id="1" name=" Chapter " dataDxfId="24"/>
+    <tableColumn id="2" name=" Discussion " dataDxfId="23"/>
+    <tableColumn id="3" name=" Exercises " dataDxfId="22"/>
+    <tableColumn id="4" name=" Problems " dataDxfId="21"/>
+    <tableColumn id="5" name=" Challenge " dataDxfId="20"/>
+    <tableColumn id="6" name=" Passage " dataDxfId="19"/>
+    <tableColumn id="7" name=" Total " dataDxfId="18">
       <calculatedColumnFormula>SUM(C7:G7)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2525,16 +2648,16 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="J6:P14" totalsRowShown="0" headerRowDxfId="9" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="J6:P14" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <autoFilter ref="J6:P14"/>
   <tableColumns count="7">
-    <tableColumn id="1" name=" Chapter " dataDxfId="17"/>
-    <tableColumn id="2" name=" Discussion " dataDxfId="16"/>
-    <tableColumn id="3" name=" Exercises " dataDxfId="15"/>
-    <tableColumn id="4" name=" Problems " dataDxfId="14"/>
-    <tableColumn id="5" name=" Challenge " dataDxfId="13"/>
-    <tableColumn id="6" name=" Passage " dataDxfId="12"/>
-    <tableColumn id="7" name=" Total " dataDxfId="11">
+    <tableColumn id="1" name=" Chapter " dataDxfId="15"/>
+    <tableColumn id="2" name=" Discussion " dataDxfId="14"/>
+    <tableColumn id="3" name=" Exercises " dataDxfId="13"/>
+    <tableColumn id="4" name=" Problems " dataDxfId="12"/>
+    <tableColumn id="5" name=" Challenge " dataDxfId="11"/>
+    <tableColumn id="6" name=" Passage " dataDxfId="10"/>
+    <tableColumn id="7" name=" Total " dataDxfId="9">
       <calculatedColumnFormula>SUM(J7:O7)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2543,26 +2666,26 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="R6:X14" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" dataCellStyle="Percent">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="R6:X14" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" dataCellStyle="Percent">
   <autoFilter ref="R6:X14"/>
   <tableColumns count="7">
-    <tableColumn id="1" name=" Chapter " dataDxfId="8"/>
-    <tableColumn id="2" name=" Discussion " dataDxfId="7" dataCellStyle="Percent">
+    <tableColumn id="1" name=" Chapter " dataDxfId="6"/>
+    <tableColumn id="2" name=" Discussion " dataDxfId="5" dataCellStyle="Percent">
       <calculatedColumnFormula>C7/K7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name=" Exercises " dataDxfId="6" dataCellStyle="Percent">
+    <tableColumn id="3" name=" Exercises " dataDxfId="4" dataCellStyle="Percent">
       <calculatedColumnFormula>D7/L7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name=" Problems " dataDxfId="5" dataCellStyle="Percent">
+    <tableColumn id="4" name=" Problems " dataDxfId="3" dataCellStyle="Percent">
       <calculatedColumnFormula>E7/M7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name=" Challenge " dataDxfId="4" dataCellStyle="Percent">
+    <tableColumn id="5" name=" Challenge " dataDxfId="2" dataCellStyle="Percent">
       <calculatedColumnFormula>F7/N7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name=" Passage " dataDxfId="3" dataCellStyle="Percent">
+    <tableColumn id="6" name=" Passage " dataDxfId="1" dataCellStyle="Percent">
       <calculatedColumnFormula>G7/O7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name=" Total " dataDxfId="2" dataCellStyle="Percent">
+    <tableColumn id="7" name=" Total " dataDxfId="0" dataCellStyle="Percent">
       <calculatedColumnFormula>H7/P7</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2835,8 +2958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:X27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2865,33 +2988,33 @@
   </cols>
   <sheetData>
     <row r="5" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="J5" s="4" t="s">
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="J5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-      <c r="R5" s="4" t="s">
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+      <c r="R5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="S5" s="4"/>
-      <c r="T5" s="4"/>
-      <c r="U5" s="4"/>
-      <c r="V5" s="4"/>
-      <c r="W5" s="4"/>
-      <c r="X5" s="4"/>
+      <c r="S5" s="10"/>
+      <c r="T5" s="10"/>
+      <c r="U5" s="10"/>
+      <c r="V5" s="10"/>
+      <c r="W5" s="10"/>
+      <c r="X5" s="10"/>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
@@ -3006,27 +3129,27 @@
       <c r="R7" s="2">
         <v>1</v>
       </c>
-      <c r="S7" s="5">
+      <c r="S7" s="4">
         <f>C7/K7</f>
         <v>1</v>
       </c>
-      <c r="T7" s="5">
+      <c r="T7" s="4">
         <f t="shared" ref="T7:X7" si="0">D7/L7</f>
         <v>1</v>
       </c>
-      <c r="U7" s="5">
+      <c r="U7" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="V7" s="5">
+      <c r="V7" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="W7" s="5">
+      <c r="W7" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="X7" s="5">
+      <c r="X7" s="4">
         <f t="shared" si="0"/>
         <v>0.61157024793388426</v>
       </c>
@@ -3081,27 +3204,27 @@
         <f>R7+1</f>
         <v>2</v>
       </c>
-      <c r="S8" s="5">
+      <c r="S8" s="4">
         <f t="shared" ref="S8:S13" si="3">C8/K8</f>
         <v>1</v>
       </c>
-      <c r="T8" s="5">
+      <c r="T8" s="4">
         <f t="shared" ref="T8:T13" si="4">D8/L8</f>
         <v>1</v>
       </c>
-      <c r="U8" s="5">
+      <c r="U8" s="4">
         <f t="shared" ref="U8:U13" si="5">E8/M8</f>
         <v>0</v>
       </c>
-      <c r="V8" s="5">
+      <c r="V8" s="4">
         <f t="shared" ref="V8:V13" si="6">F8/N8</f>
         <v>0</v>
       </c>
-      <c r="W8" s="5">
+      <c r="W8" s="4">
         <f t="shared" ref="W8:W13" si="7">G8/O8</f>
         <v>0</v>
       </c>
-      <c r="X8" s="5">
+      <c r="X8" s="4">
         <f t="shared" ref="X8:X13" si="8">H8/P8</f>
         <v>0.65517241379310343</v>
       </c>
@@ -3131,7 +3254,7 @@
         <v>54</v>
       </c>
       <c r="J9" s="2">
-        <f t="shared" ref="J9:J14" si="9">J8+1</f>
+        <f t="shared" ref="J9:J13" si="9">J8+1</f>
         <v>3</v>
       </c>
       <c r="K9" s="2">
@@ -3157,27 +3280,27 @@
         <f t="shared" ref="R9:R13" si="10">R8+1</f>
         <v>3</v>
       </c>
-      <c r="S9" s="5">
+      <c r="S9" s="4">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="T9" s="5">
+      <c r="T9" s="4">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="U9" s="5">
+      <c r="U9" s="4">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="V9" s="5">
+      <c r="V9" s="4">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="W9" s="5">
+      <c r="W9" s="4">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="X9" s="5">
+      <c r="X9" s="4">
         <f t="shared" si="8"/>
         <v>0.52427184466019416</v>
       </c>
@@ -3233,27 +3356,27 @@
         <f t="shared" si="10"/>
         <v>4</v>
       </c>
-      <c r="S10" s="5">
+      <c r="S10" s="4">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="T10" s="5">
+      <c r="T10" s="4">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="U10" s="5">
+      <c r="U10" s="4">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="V10" s="5">
+      <c r="V10" s="4">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="W10" s="5">
+      <c r="W10" s="4">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="X10" s="5">
+      <c r="X10" s="4">
         <f t="shared" si="8"/>
         <v>0.65686274509803921</v>
       </c>
@@ -3267,7 +3390,7 @@
         <v>28</v>
       </c>
       <c r="D11" s="2">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="E11" s="2">
         <v>0</v>
@@ -3280,7 +3403,7 @@
       </c>
       <c r="H11" s="2">
         <f t="shared" si="1"/>
-        <v>53</v>
+        <v>87</v>
       </c>
       <c r="J11" s="2">
         <f t="shared" si="9"/>
@@ -3309,29 +3432,29 @@
         <f t="shared" si="10"/>
         <v>5</v>
       </c>
-      <c r="S11" s="5">
+      <c r="S11" s="4">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="T11" s="5">
+      <c r="T11" s="4">
         <f t="shared" si="4"/>
-        <v>0.42372881355932202</v>
-      </c>
-      <c r="U11" s="5">
+        <v>1</v>
+      </c>
+      <c r="U11" s="4">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="V11" s="5">
+      <c r="V11" s="4">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="W11" s="5">
+      <c r="W11" s="4">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="X11" s="5">
+      <c r="X11" s="4">
         <f t="shared" si="8"/>
-        <v>0.35099337748344372</v>
+        <v>0.57615894039735094</v>
       </c>
     </row>
     <row r="12" spans="2:24" x14ac:dyDescent="0.25">
@@ -3340,10 +3463,10 @@
         <v>6</v>
       </c>
       <c r="C12" s="2">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D12" s="2">
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="E12" s="2">
         <v>0</v>
@@ -3356,7 +3479,7 @@
       </c>
       <c r="H12" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="J12" s="2">
         <f t="shared" si="9"/>
@@ -3385,29 +3508,29 @@
         <f t="shared" si="10"/>
         <v>6</v>
       </c>
-      <c r="S12" s="5">
+      <c r="S12" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="T12" s="5">
+        <v>1</v>
+      </c>
+      <c r="T12" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="U12" s="5">
+        <v>1</v>
+      </c>
+      <c r="U12" s="4">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="V12" s="5">
+      <c r="V12" s="4">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="W12" s="5">
+      <c r="W12" s="4">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="X12" s="5">
+      <c r="X12" s="4">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>0.6692913385826772</v>
       </c>
     </row>
     <row r="13" spans="2:24" x14ac:dyDescent="0.25">
@@ -3416,10 +3539,10 @@
         <v>7</v>
       </c>
       <c r="C13" s="2">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D13" s="2">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="E13" s="2">
         <v>0</v>
@@ -3432,7 +3555,7 @@
       </c>
       <c r="H13" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="J13" s="2">
         <f t="shared" si="9"/>
@@ -3461,29 +3584,29 @@
         <f t="shared" si="10"/>
         <v>7</v>
       </c>
-      <c r="S13" s="5">
+      <c r="S13" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="T13" s="5">
+        <v>1</v>
+      </c>
+      <c r="T13" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="U13" s="5">
+        <v>1</v>
+      </c>
+      <c r="U13" s="4">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="V13" s="5">
+      <c r="V13" s="4">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="W13" s="5">
+      <c r="W13" s="4">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="X13" s="5">
+      <c r="X13" s="4">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>0.51754385964912286</v>
       </c>
     </row>
     <row r="14" spans="2:24" x14ac:dyDescent="0.25">
@@ -3492,11 +3615,11 @@
       </c>
       <c r="C14" s="2">
         <f>SUM(C7:C13)</f>
-        <v>130</v>
+        <v>177</v>
       </c>
       <c r="D14" s="2">
         <f>SUM(D7:D13)</f>
-        <v>194</v>
+        <v>325</v>
       </c>
       <c r="E14" s="2">
         <f>SUM(E7:E13)</f>
@@ -3512,7 +3635,7 @@
       </c>
       <c r="H14" s="2">
         <f>SUM(C14:G14)</f>
-        <v>324</v>
+        <v>502</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>7</v>
@@ -3544,29 +3667,29 @@
       <c r="R14" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="S14" s="5">
+      <c r="S14" s="4">
         <f t="shared" ref="S14" si="13">C14/K14</f>
-        <v>0.7344632768361582</v>
-      </c>
-      <c r="T14" s="5">
+        <v>1</v>
+      </c>
+      <c r="T14" s="4">
         <f t="shared" ref="T14" si="14">D14/L14</f>
-        <v>0.59692307692307689</v>
-      </c>
-      <c r="U14" s="5">
+        <v>1</v>
+      </c>
+      <c r="U14" s="4">
         <f t="shared" ref="U14" si="15">E14/M14</f>
         <v>0</v>
       </c>
-      <c r="V14" s="5">
+      <c r="V14" s="4">
         <f t="shared" ref="V14" si="16">F14/N14</f>
         <v>0</v>
       </c>
-      <c r="W14" s="5">
+      <c r="W14" s="4">
         <f t="shared" ref="W14" si="17">G14/O14</f>
         <v>0</v>
       </c>
-      <c r="X14" s="5">
+      <c r="X14" s="4">
         <f t="shared" ref="X14" si="18">H14/P14</f>
-        <v>0.40198511166253104</v>
+        <v>0.62282878411910669</v>
       </c>
     </row>
     <row r="15" spans="2:24" x14ac:dyDescent="0.25">
@@ -3576,24 +3699,24 @@
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="J17" s="4" t="s">
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="J17" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
-      <c r="P17" s="4"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="10"/>
     </row>
     <row r="18" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
@@ -3617,25 +3740,25 @@
       <c r="H18" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J18" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="K18" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="L18" s="7" t="s">
+      <c r="J18" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="K18" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="L18" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="M18" s="7" t="s">
+      <c r="M18" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="N18" s="7" t="s">
+      <c r="N18" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="O18" s="7" t="s">
+      <c r="O18" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="P18" s="8" t="s">
+      <c r="P18" s="7" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3670,28 +3793,28 @@
       <c r="J19" s="2">
         <v>1</v>
       </c>
-      <c r="K19" s="9">
-        <f>K7/K$14</f>
+      <c r="K19" s="8">
+        <f t="shared" ref="K19:P19" si="20">K7/K$14</f>
         <v>0.14689265536723164</v>
       </c>
-      <c r="L19" s="9">
-        <f>L7/L$14</f>
+      <c r="L19" s="8">
+        <f t="shared" si="20"/>
         <v>0.14769230769230771</v>
       </c>
-      <c r="M19" s="9">
-        <f>M7/M$14</f>
+      <c r="M19" s="8">
+        <f t="shared" si="20"/>
         <v>0.15471698113207547</v>
       </c>
-      <c r="N19" s="9">
-        <f>N7/N$14</f>
+      <c r="N19" s="8">
+        <f t="shared" si="20"/>
         <v>0.125</v>
       </c>
-      <c r="O19" s="9">
-        <f>O7/O$14</f>
+      <c r="O19" s="8">
+        <f t="shared" si="20"/>
         <v>0.13043478260869565</v>
       </c>
-      <c r="P19" s="9">
-        <f>P7/P$14</f>
+      <c r="P19" s="8">
+        <f t="shared" si="20"/>
         <v>0.15012406947890819</v>
       </c>
     </row>
@@ -3701,339 +3824,339 @@
         <v>2</v>
       </c>
       <c r="C20" s="2">
-        <f t="shared" ref="C20:G20" si="20">K8-C8</f>
+        <f t="shared" ref="C20:G20" si="21">K8-C8</f>
         <v>0</v>
       </c>
       <c r="D20" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="E20" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>32</v>
       </c>
       <c r="F20" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>3</v>
       </c>
       <c r="G20" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>3</v>
       </c>
       <c r="H20" s="2">
-        <f t="shared" ref="H20:H26" si="21">SUM(B20:G20)</f>
+        <f t="shared" ref="H20:H26" si="22">SUM(B20:G20)</f>
         <v>40</v>
       </c>
       <c r="J20" s="2">
         <v>2</v>
       </c>
-      <c r="K20" s="9">
-        <f t="shared" ref="K20:L25" si="22">K8/K$14</f>
+      <c r="K20" s="8">
+        <f t="shared" ref="K20:L25" si="23">K8/K$14</f>
         <v>0.12429378531073447</v>
       </c>
-      <c r="L20" s="9">
-        <f t="shared" si="22"/>
+      <c r="L20" s="8">
+        <f t="shared" si="23"/>
         <v>0.16615384615384615</v>
       </c>
-      <c r="M20" s="9">
-        <f t="shared" ref="M20:P20" si="23">M8/M$14</f>
+      <c r="M20" s="8">
+        <f t="shared" ref="M20:P20" si="24">M8/M$14</f>
         <v>0.12075471698113208</v>
       </c>
-      <c r="N20" s="9">
-        <f t="shared" si="23"/>
+      <c r="N20" s="8">
+        <f t="shared" si="24"/>
         <v>0.1875</v>
       </c>
-      <c r="O20" s="9">
-        <f t="shared" si="23"/>
+      <c r="O20" s="8">
+        <f t="shared" si="24"/>
         <v>0.13043478260869565</v>
       </c>
-      <c r="P20" s="9">
-        <f t="shared" si="23"/>
+      <c r="P20" s="8">
+        <f t="shared" si="24"/>
         <v>0.14392059553349876</v>
       </c>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B21" s="2">
-        <f t="shared" ref="B21:B26" si="24">B20+1</f>
+        <f t="shared" ref="B21:B25" si="25">B20+1</f>
         <v>3</v>
       </c>
       <c r="C21" s="2">
-        <f t="shared" ref="C21:G21" si="25">K9-C9</f>
+        <f t="shared" ref="C21:G21" si="26">K9-C9</f>
         <v>0</v>
       </c>
       <c r="D21" s="2">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="E21" s="2">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>40</v>
       </c>
       <c r="F21" s="2">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>3</v>
       </c>
       <c r="G21" s="2">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>3</v>
       </c>
       <c r="H21" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>49</v>
       </c>
       <c r="J21" s="2">
         <v>3</v>
       </c>
-      <c r="K21" s="9">
-        <f t="shared" si="22"/>
+      <c r="K21" s="8">
+        <f t="shared" si="23"/>
         <v>9.03954802259887E-2</v>
       </c>
-      <c r="L21" s="9">
-        <f t="shared" si="22"/>
+      <c r="L21" s="8">
+        <f t="shared" si="23"/>
         <v>0.11692307692307692</v>
       </c>
-      <c r="M21" s="9">
-        <f t="shared" ref="M21:P21" si="26">M9/M$14</f>
+      <c r="M21" s="8">
+        <f t="shared" ref="M21:P21" si="27">M9/M$14</f>
         <v>0.15094339622641509</v>
       </c>
-      <c r="N21" s="9">
-        <f t="shared" si="26"/>
+      <c r="N21" s="8">
+        <f t="shared" si="27"/>
         <v>0.1875</v>
       </c>
-      <c r="O21" s="9">
-        <f t="shared" si="26"/>
+      <c r="O21" s="8">
+        <f t="shared" si="27"/>
         <v>0.13043478260869565</v>
       </c>
-      <c r="P21" s="9">
-        <f t="shared" si="26"/>
+      <c r="P21" s="8">
+        <f t="shared" si="27"/>
         <v>0.12779156327543426</v>
       </c>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B22" s="2">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>4</v>
       </c>
       <c r="C22" s="2">
-        <f t="shared" ref="C22:G22" si="27">K10-C10</f>
+        <f t="shared" ref="C22:G22" si="28">K10-C10</f>
         <v>0</v>
       </c>
       <c r="D22" s="2">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="E22" s="2">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>26</v>
       </c>
       <c r="F22" s="2">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>1</v>
       </c>
       <c r="G22" s="2">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>4</v>
       </c>
       <c r="H22" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>35</v>
       </c>
       <c r="J22" s="2">
         <v>4</v>
       </c>
-      <c r="K22" s="9">
-        <f t="shared" si="22"/>
+      <c r="K22" s="8">
+        <f t="shared" si="23"/>
         <v>0.21468926553672316</v>
       </c>
-      <c r="L22" s="9">
-        <f t="shared" si="22"/>
+      <c r="L22" s="8">
+        <f t="shared" si="23"/>
         <v>8.9230769230769225E-2</v>
       </c>
-      <c r="M22" s="9">
-        <f t="shared" ref="M22:P22" si="28">M10/M$14</f>
+      <c r="M22" s="8">
+        <f t="shared" ref="M22:P22" si="29">M10/M$14</f>
         <v>9.8113207547169817E-2</v>
       </c>
-      <c r="N22" s="9">
-        <f t="shared" si="28"/>
+      <c r="N22" s="8">
+        <f t="shared" si="29"/>
         <v>6.25E-2</v>
       </c>
-      <c r="O22" s="9">
-        <f t="shared" si="28"/>
+      <c r="O22" s="8">
+        <f t="shared" si="29"/>
         <v>0.17391304347826086</v>
       </c>
-      <c r="P22" s="9">
-        <f t="shared" si="28"/>
+      <c r="P22" s="8">
+        <f t="shared" si="29"/>
         <v>0.12655086848635236</v>
       </c>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B23" s="2">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>5</v>
       </c>
       <c r="C23" s="2">
-        <f t="shared" ref="C23:G23" si="29">K11-C11</f>
+        <f t="shared" ref="C23:G23" si="30">K11-C11</f>
         <v>0</v>
       </c>
       <c r="D23" s="2">
-        <f t="shared" si="29"/>
-        <v>34</v>
+        <f t="shared" si="30"/>
+        <v>0</v>
       </c>
       <c r="E23" s="2">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>52</v>
       </c>
       <c r="F23" s="2">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>4</v>
       </c>
       <c r="G23" s="2">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>3</v>
       </c>
       <c r="H23" s="2">
-        <f t="shared" si="21"/>
-        <v>98</v>
-      </c>
-      <c r="J23" s="10">
+        <f t="shared" si="22"/>
+        <v>64</v>
+      </c>
+      <c r="J23" s="9">
         <v>5</v>
       </c>
-      <c r="K23" s="9">
-        <f t="shared" si="22"/>
+      <c r="K23" s="8">
+        <f t="shared" si="23"/>
         <v>0.15819209039548024</v>
       </c>
-      <c r="L23" s="9">
-        <f t="shared" si="22"/>
+      <c r="L23" s="8">
+        <f t="shared" si="23"/>
         <v>0.18153846153846154</v>
       </c>
-      <c r="M23" s="9">
-        <f t="shared" ref="M23:P23" si="30">M11/M$14</f>
+      <c r="M23" s="8">
+        <f t="shared" ref="M23:P23" si="31">M11/M$14</f>
         <v>0.19622641509433963</v>
       </c>
-      <c r="N23" s="9">
-        <f t="shared" si="30"/>
+      <c r="N23" s="8">
+        <f t="shared" si="31"/>
         <v>0.25</v>
       </c>
-      <c r="O23" s="9">
-        <f t="shared" si="30"/>
+      <c r="O23" s="8">
+        <f t="shared" si="31"/>
         <v>0.13043478260869565</v>
       </c>
-      <c r="P23" s="9">
-        <f t="shared" si="30"/>
+      <c r="P23" s="8">
+        <f t="shared" si="31"/>
         <v>0.18734491315136476</v>
       </c>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B24" s="2">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>6</v>
       </c>
       <c r="C24" s="2">
-        <f t="shared" ref="C24:G24" si="31">K12-C12</f>
-        <v>24</v>
+        <f t="shared" ref="C24:G24" si="32">K12-C12</f>
+        <v>0</v>
       </c>
       <c r="D24" s="2">
-        <f t="shared" si="31"/>
-        <v>61</v>
+        <f t="shared" si="32"/>
+        <v>0</v>
       </c>
       <c r="E24" s="2">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>31</v>
       </c>
       <c r="F24" s="2">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>2</v>
       </c>
       <c r="G24" s="2">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>3</v>
       </c>
       <c r="H24" s="2">
-        <f t="shared" si="21"/>
-        <v>127</v>
+        <f t="shared" si="22"/>
+        <v>42</v>
       </c>
       <c r="J24" s="2">
         <v>6</v>
       </c>
-      <c r="K24" s="9">
-        <f t="shared" si="22"/>
+      <c r="K24" s="8">
+        <f t="shared" si="23"/>
         <v>0.13559322033898305</v>
       </c>
-      <c r="L24" s="9">
-        <f t="shared" si="22"/>
+      <c r="L24" s="8">
+        <f t="shared" si="23"/>
         <v>0.18769230769230769</v>
       </c>
-      <c r="M24" s="9">
-        <f t="shared" ref="M24:P24" si="32">M12/M$14</f>
+      <c r="M24" s="8">
+        <f t="shared" ref="M24:P24" si="33">M12/M$14</f>
         <v>0.1169811320754717</v>
       </c>
-      <c r="N24" s="9">
-        <f t="shared" si="32"/>
+      <c r="N24" s="8">
+        <f t="shared" si="33"/>
         <v>0.125</v>
       </c>
-      <c r="O24" s="9">
-        <f t="shared" si="32"/>
+      <c r="O24" s="8">
+        <f t="shared" si="33"/>
         <v>0.13043478260869565</v>
       </c>
-      <c r="P24" s="9">
-        <f t="shared" si="32"/>
+      <c r="P24" s="8">
+        <f t="shared" si="33"/>
         <v>0.15756823821339949</v>
       </c>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B25" s="2">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>7</v>
       </c>
       <c r="C25" s="2">
-        <f t="shared" ref="C25:G25" si="33">K13-C13</f>
-        <v>23</v>
+        <f t="shared" ref="C25:G25" si="34">K13-C13</f>
+        <v>0</v>
       </c>
       <c r="D25" s="2">
-        <f t="shared" si="33"/>
-        <v>36</v>
+        <f t="shared" si="34"/>
+        <v>0</v>
       </c>
       <c r="E25" s="2">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>43</v>
       </c>
       <c r="F25" s="2">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="G25" s="2">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>4</v>
       </c>
       <c r="H25" s="2">
-        <f t="shared" si="21"/>
-        <v>114</v>
+        <f t="shared" si="22"/>
+        <v>55</v>
       </c>
       <c r="J25" s="2">
         <v>7</v>
       </c>
-      <c r="K25" s="9">
-        <f t="shared" si="22"/>
+      <c r="K25" s="8">
+        <f t="shared" si="23"/>
         <v>0.12994350282485875</v>
       </c>
-      <c r="L25" s="9">
-        <f t="shared" si="22"/>
+      <c r="L25" s="8">
+        <f t="shared" si="23"/>
         <v>0.11076923076923077</v>
       </c>
-      <c r="M25" s="9">
-        <f t="shared" ref="M25:P25" si="34">M13/M$14</f>
+      <c r="M25" s="8">
+        <f t="shared" ref="M25:P25" si="35">M13/M$14</f>
         <v>0.16226415094339622</v>
       </c>
-      <c r="N25" s="9">
-        <f t="shared" si="34"/>
+      <c r="N25" s="8">
+        <f t="shared" si="35"/>
         <v>6.25E-2</v>
       </c>
-      <c r="O25" s="9">
-        <f t="shared" si="34"/>
+      <c r="O25" s="8">
+        <f t="shared" si="35"/>
         <v>0.17391304347826086</v>
       </c>
-      <c r="P25" s="9">
-        <f t="shared" si="34"/>
+      <c r="P25" s="8">
+        <f t="shared" si="35"/>
         <v>0.14143920595533499</v>
       </c>
     </row>
@@ -4043,52 +4166,52 @@
       </c>
       <c r="C26" s="2">
         <f>SUM(C19:C25)</f>
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="D26" s="2">
-        <f t="shared" ref="D26" si="35">SUM(D19:D25)</f>
-        <v>131</v>
+        <f t="shared" ref="D26" si="36">SUM(D19:D25)</f>
+        <v>0</v>
       </c>
       <c r="E26" s="2">
-        <f t="shared" ref="E26" si="36">SUM(E19:E25)</f>
+        <f t="shared" ref="E26" si="37">SUM(E19:E25)</f>
         <v>265</v>
       </c>
       <c r="F26" s="2">
-        <f t="shared" ref="F26" si="37">SUM(F19:F25)</f>
+        <f t="shared" ref="F26" si="38">SUM(F19:F25)</f>
         <v>16</v>
       </c>
       <c r="G26" s="2">
-        <f t="shared" ref="G26" si="38">SUM(G19:G25)</f>
+        <f t="shared" ref="G26" si="39">SUM(G19:G25)</f>
         <v>23</v>
       </c>
       <c r="H26" s="2">
-        <f t="shared" si="21"/>
-        <v>482</v>
+        <f t="shared" si="22"/>
+        <v>304</v>
       </c>
       <c r="J26" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K26" s="9">
+      <c r="K26" s="8">
         <f>K14/$P$14</f>
         <v>0.21960297766749379</v>
       </c>
-      <c r="L26" s="9">
-        <f t="shared" ref="L26:O26" si="39">L14/$P$14</f>
+      <c r="L26" s="8">
+        <f t="shared" ref="L26:O26" si="40">L14/$P$14</f>
         <v>0.40322580645161288</v>
       </c>
-      <c r="M26" s="9">
-        <f t="shared" si="39"/>
+      <c r="M26" s="8">
+        <f t="shared" si="40"/>
         <v>0.32878411910669975</v>
       </c>
-      <c r="N26" s="9">
-        <f t="shared" si="39"/>
+      <c r="N26" s="8">
+        <f t="shared" si="40"/>
         <v>1.9851116625310174E-2</v>
       </c>
-      <c r="O26" s="9">
-        <f t="shared" si="39"/>
+      <c r="O26" s="8">
+        <f t="shared" si="40"/>
         <v>2.8535980148883373E-2</v>
       </c>
-      <c r="P26" s="9">
+      <c r="P26" s="8">
         <f>P14/$P$14</f>
         <v>1</v>
       </c>
@@ -4201,4 +4324,1514 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="D4:R32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" customWidth="1"/>
+    <col min="9" max="9" width="11" customWidth="1"/>
+    <col min="12" max="12" width="11" customWidth="1"/>
+    <col min="13" max="13" width="13.28515625" customWidth="1"/>
+    <col min="14" max="14" width="12.140625" customWidth="1"/>
+    <col min="15" max="15" width="12.42578125" customWidth="1"/>
+    <col min="16" max="16" width="12.85546875" customWidth="1"/>
+    <col min="17" max="17" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D4" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="L4" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="11"/>
+    </row>
+    <row r="5" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D5" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="L5" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="M5" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="N5" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="O5" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="P5" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q5" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="R5" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D6" s="15">
+        <v>8</v>
+      </c>
+      <c r="E6" s="16">
+        <v>26</v>
+      </c>
+      <c r="F6" s="16">
+        <v>63</v>
+      </c>
+      <c r="G6" s="16">
+        <v>39</v>
+      </c>
+      <c r="H6" s="16">
+        <v>3</v>
+      </c>
+      <c r="I6" s="16">
+        <v>4</v>
+      </c>
+      <c r="J6" s="17">
+        <f>SUM(E6:I6)</f>
+        <v>135</v>
+      </c>
+      <c r="L6" s="15">
+        <v>8</v>
+      </c>
+      <c r="M6" s="16">
+        <v>0</v>
+      </c>
+      <c r="N6" s="16">
+        <v>0</v>
+      </c>
+      <c r="O6" s="16">
+        <v>0</v>
+      </c>
+      <c r="P6" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="16">
+        <v>0</v>
+      </c>
+      <c r="R6" s="17">
+        <f>SUM(M6:Q6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D7" s="15">
+        <v>9</v>
+      </c>
+      <c r="E7" s="16">
+        <v>22</v>
+      </c>
+      <c r="F7" s="16">
+        <v>55</v>
+      </c>
+      <c r="G7" s="16">
+        <v>34</v>
+      </c>
+      <c r="H7" s="16">
+        <v>2</v>
+      </c>
+      <c r="I7" s="16">
+        <v>4</v>
+      </c>
+      <c r="J7" s="17">
+        <f t="shared" ref="J7:J11" si="0">SUM(E7:I7)</f>
+        <v>117</v>
+      </c>
+      <c r="L7" s="15">
+        <v>9</v>
+      </c>
+      <c r="M7" s="16">
+        <v>0</v>
+      </c>
+      <c r="N7" s="16">
+        <v>0</v>
+      </c>
+      <c r="O7" s="16">
+        <v>0</v>
+      </c>
+      <c r="P7" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="16">
+        <v>0</v>
+      </c>
+      <c r="R7" s="17">
+        <f t="shared" ref="R7:R11" si="1">SUM(M7:Q7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D8" s="15">
+        <v>10</v>
+      </c>
+      <c r="E8" s="16">
+        <v>30</v>
+      </c>
+      <c r="F8" s="16">
+        <v>53</v>
+      </c>
+      <c r="G8" s="16">
+        <v>37</v>
+      </c>
+      <c r="H8" s="16">
+        <v>3</v>
+      </c>
+      <c r="I8" s="16">
+        <v>4</v>
+      </c>
+      <c r="J8" s="17">
+        <f t="shared" si="0"/>
+        <v>127</v>
+      </c>
+      <c r="L8" s="15">
+        <v>10</v>
+      </c>
+      <c r="M8" s="16">
+        <v>0</v>
+      </c>
+      <c r="N8" s="16">
+        <v>0</v>
+      </c>
+      <c r="O8" s="16">
+        <v>0</v>
+      </c>
+      <c r="P8" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="16">
+        <v>0</v>
+      </c>
+      <c r="R8" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D9" s="15">
+        <v>11</v>
+      </c>
+      <c r="E9" s="16">
+        <v>25</v>
+      </c>
+      <c r="F9" s="16">
+        <v>41</v>
+      </c>
+      <c r="G9" s="16">
+        <v>47</v>
+      </c>
+      <c r="H9" s="16">
+        <v>3</v>
+      </c>
+      <c r="I9" s="16">
+        <v>4</v>
+      </c>
+      <c r="J9" s="17">
+        <f t="shared" si="0"/>
+        <v>120</v>
+      </c>
+      <c r="L9" s="15">
+        <v>11</v>
+      </c>
+      <c r="M9" s="16">
+        <v>0</v>
+      </c>
+      <c r="N9" s="16">
+        <v>0</v>
+      </c>
+      <c r="O9" s="16">
+        <v>0</v>
+      </c>
+      <c r="P9" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="16">
+        <v>0</v>
+      </c>
+      <c r="R9" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D10" s="15">
+        <v>12</v>
+      </c>
+      <c r="E10" s="16">
+        <v>30</v>
+      </c>
+      <c r="F10" s="16">
+        <v>50</v>
+      </c>
+      <c r="G10" s="16">
+        <v>37</v>
+      </c>
+      <c r="H10" s="16">
+        <v>1</v>
+      </c>
+      <c r="I10" s="16">
+        <v>4</v>
+      </c>
+      <c r="J10" s="17">
+        <f t="shared" si="0"/>
+        <v>122</v>
+      </c>
+      <c r="L10" s="15">
+        <v>12</v>
+      </c>
+      <c r="M10" s="16">
+        <v>0</v>
+      </c>
+      <c r="N10" s="16">
+        <v>0</v>
+      </c>
+      <c r="O10" s="16">
+        <v>0</v>
+      </c>
+      <c r="P10" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="16">
+        <v>0</v>
+      </c>
+      <c r="R10" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D11" s="15">
+        <v>13</v>
+      </c>
+      <c r="E11" s="16">
+        <v>21</v>
+      </c>
+      <c r="F11" s="16">
+        <v>40</v>
+      </c>
+      <c r="G11" s="16">
+        <v>38</v>
+      </c>
+      <c r="H11" s="16">
+        <v>3</v>
+      </c>
+      <c r="I11" s="16">
+        <v>3</v>
+      </c>
+      <c r="J11" s="17">
+        <f t="shared" si="0"/>
+        <v>105</v>
+      </c>
+      <c r="L11" s="15">
+        <v>13</v>
+      </c>
+      <c r="M11" s="16">
+        <v>0</v>
+      </c>
+      <c r="N11" s="16">
+        <v>0</v>
+      </c>
+      <c r="O11" s="16">
+        <v>0</v>
+      </c>
+      <c r="P11" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="16">
+        <v>0</v>
+      </c>
+      <c r="R11" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D12" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="19">
+        <f>SUM(E6:E11)</f>
+        <v>154</v>
+      </c>
+      <c r="F12" s="19">
+        <f>SUM(F6:F11)</f>
+        <v>302</v>
+      </c>
+      <c r="G12" s="19">
+        <f>SUM(G6:G11)</f>
+        <v>232</v>
+      </c>
+      <c r="H12" s="19">
+        <f>SUM(H6:H11)</f>
+        <v>15</v>
+      </c>
+      <c r="I12" s="19">
+        <f>SUM(I6:I11)</f>
+        <v>23</v>
+      </c>
+      <c r="J12" s="19">
+        <f>SUM(J6:J11)</f>
+        <v>726</v>
+      </c>
+      <c r="L12" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="M12" s="19">
+        <f>SUM(M6:M11)</f>
+        <v>0</v>
+      </c>
+      <c r="N12" s="19">
+        <f>SUM(N6:N11)</f>
+        <v>0</v>
+      </c>
+      <c r="O12" s="19">
+        <f>SUM(O6:O11)</f>
+        <v>0</v>
+      </c>
+      <c r="P12" s="19">
+        <f>SUM(P6:P11)</f>
+        <v>0</v>
+      </c>
+      <c r="Q12" s="19">
+        <f>SUM(Q6:Q11)</f>
+        <v>0</v>
+      </c>
+      <c r="R12" s="19">
+        <f>SUM(R6:R11)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D14" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="L14" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="11"/>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="11"/>
+      <c r="R14" s="11"/>
+    </row>
+    <row r="15" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D15" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="I15" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="J15" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="L15" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="M15" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="N15" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="O15" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="P15" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q15" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="R15" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D16" s="15">
+        <v>8</v>
+      </c>
+      <c r="E16" s="22">
+        <f>M6/E6</f>
+        <v>0</v>
+      </c>
+      <c r="F16" s="22">
+        <f>N6/F6</f>
+        <v>0</v>
+      </c>
+      <c r="G16" s="22">
+        <f>O6/G6</f>
+        <v>0</v>
+      </c>
+      <c r="H16" s="22">
+        <f>P6/H6</f>
+        <v>0</v>
+      </c>
+      <c r="I16" s="22">
+        <f>Q6/I6</f>
+        <v>0</v>
+      </c>
+      <c r="J16" s="23">
+        <f>R6/J6</f>
+        <v>0</v>
+      </c>
+      <c r="L16" s="15">
+        <v>8</v>
+      </c>
+      <c r="M16" s="22">
+        <f>1-E16</f>
+        <v>1</v>
+      </c>
+      <c r="N16" s="22">
+        <f t="shared" ref="N16:N22" si="2">1-F16</f>
+        <v>1</v>
+      </c>
+      <c r="O16" s="22">
+        <f t="shared" ref="O16:O22" si="3">1-G16</f>
+        <v>1</v>
+      </c>
+      <c r="P16" s="22">
+        <f t="shared" ref="P16:P22" si="4">1-H16</f>
+        <v>1</v>
+      </c>
+      <c r="Q16" s="22">
+        <f t="shared" ref="Q16:Q22" si="5">1-I16</f>
+        <v>1</v>
+      </c>
+      <c r="R16" s="23">
+        <f t="shared" ref="R16:R22" si="6">1-J16</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D17" s="15">
+        <v>9</v>
+      </c>
+      <c r="E17" s="22">
+        <f>M7/E7</f>
+        <v>0</v>
+      </c>
+      <c r="F17" s="22">
+        <f>N7/F7</f>
+        <v>0</v>
+      </c>
+      <c r="G17" s="22">
+        <f>O7/G7</f>
+        <v>0</v>
+      </c>
+      <c r="H17" s="22">
+        <f>P7/H7</f>
+        <v>0</v>
+      </c>
+      <c r="I17" s="22">
+        <f>Q7/I7</f>
+        <v>0</v>
+      </c>
+      <c r="J17" s="23">
+        <f>R7/J7</f>
+        <v>0</v>
+      </c>
+      <c r="L17" s="15">
+        <v>9</v>
+      </c>
+      <c r="M17" s="22">
+        <f t="shared" ref="M17:M22" si="7">1-E17</f>
+        <v>1</v>
+      </c>
+      <c r="N17" s="22">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O17" s="22">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P17" s="22">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="Q17" s="22">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="R17" s="23">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D18" s="15">
+        <v>10</v>
+      </c>
+      <c r="E18" s="22">
+        <f>M8/E8</f>
+        <v>0</v>
+      </c>
+      <c r="F18" s="22">
+        <f>N8/F8</f>
+        <v>0</v>
+      </c>
+      <c r="G18" s="22">
+        <f>O8/G8</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="22">
+        <f>P8/H8</f>
+        <v>0</v>
+      </c>
+      <c r="I18" s="22">
+        <f>Q8/I8</f>
+        <v>0</v>
+      </c>
+      <c r="J18" s="23">
+        <f>R8/J8</f>
+        <v>0</v>
+      </c>
+      <c r="L18" s="15">
+        <v>10</v>
+      </c>
+      <c r="M18" s="22">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="N18" s="22">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O18" s="22">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P18" s="22">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="Q18" s="22">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="R18" s="23">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D19" s="15">
+        <v>11</v>
+      </c>
+      <c r="E19" s="22">
+        <f>M9/E9</f>
+        <v>0</v>
+      </c>
+      <c r="F19" s="22">
+        <f>N9/F9</f>
+        <v>0</v>
+      </c>
+      <c r="G19" s="22">
+        <f>O9/G9</f>
+        <v>0</v>
+      </c>
+      <c r="H19" s="22">
+        <f>P9/H9</f>
+        <v>0</v>
+      </c>
+      <c r="I19" s="22">
+        <f>Q9/I9</f>
+        <v>0</v>
+      </c>
+      <c r="J19" s="23">
+        <f>R9/J9</f>
+        <v>0</v>
+      </c>
+      <c r="L19" s="15">
+        <v>11</v>
+      </c>
+      <c r="M19" s="22">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="N19" s="22">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O19" s="22">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P19" s="22">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="Q19" s="22">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="R19" s="23">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D20" s="15">
+        <v>12</v>
+      </c>
+      <c r="E20" s="22">
+        <f>M10/E10</f>
+        <v>0</v>
+      </c>
+      <c r="F20" s="22">
+        <f>N10/F10</f>
+        <v>0</v>
+      </c>
+      <c r="G20" s="22">
+        <f>O10/G10</f>
+        <v>0</v>
+      </c>
+      <c r="H20" s="22">
+        <f>P10/H10</f>
+        <v>0</v>
+      </c>
+      <c r="I20" s="22">
+        <f>Q10/I10</f>
+        <v>0</v>
+      </c>
+      <c r="J20" s="23">
+        <f>R10/J10</f>
+        <v>0</v>
+      </c>
+      <c r="L20" s="15">
+        <v>12</v>
+      </c>
+      <c r="M20" s="22">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="N20" s="22">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O20" s="22">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P20" s="22">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="Q20" s="22">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="R20" s="23">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D21" s="15">
+        <v>13</v>
+      </c>
+      <c r="E21" s="22">
+        <f>M11/E11</f>
+        <v>0</v>
+      </c>
+      <c r="F21" s="22">
+        <f>N11/F11</f>
+        <v>0</v>
+      </c>
+      <c r="G21" s="22">
+        <f>O11/G11</f>
+        <v>0</v>
+      </c>
+      <c r="H21" s="22">
+        <f>P11/H11</f>
+        <v>0</v>
+      </c>
+      <c r="I21" s="22">
+        <f>Q11/I11</f>
+        <v>0</v>
+      </c>
+      <c r="J21" s="23">
+        <f>R11/J11</f>
+        <v>0</v>
+      </c>
+      <c r="L21" s="15">
+        <v>13</v>
+      </c>
+      <c r="M21" s="22">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="N21" s="22">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O21" s="22">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P21" s="22">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="Q21" s="22">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="R21" s="23">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D22" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="24">
+        <f>M12/E12</f>
+        <v>0</v>
+      </c>
+      <c r="F22" s="24">
+        <f>N12/F12</f>
+        <v>0</v>
+      </c>
+      <c r="G22" s="24">
+        <f>O12/G12</f>
+        <v>0</v>
+      </c>
+      <c r="H22" s="24">
+        <f>P12/H12</f>
+        <v>0</v>
+      </c>
+      <c r="I22" s="24">
+        <f>Q12/I12</f>
+        <v>0</v>
+      </c>
+      <c r="J22" s="24">
+        <f>R12/J12</f>
+        <v>0</v>
+      </c>
+      <c r="L22" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="M22" s="24">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="N22" s="24">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O22" s="24">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P22" s="24">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="Q22" s="24">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="R22" s="24">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D24" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="L24" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="M24" s="11"/>
+      <c r="N24" s="11"/>
+      <c r="O24" s="11"/>
+      <c r="P24" s="11"/>
+      <c r="Q24" s="11"/>
+      <c r="R24" s="11"/>
+    </row>
+    <row r="25" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D25" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="H25" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="I25" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="J25" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="L25" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="M25" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="N25" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="O25" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="P25" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q25" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="R25" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D26" s="15">
+        <v>8</v>
+      </c>
+      <c r="E26" s="20">
+        <f>E6/E$12</f>
+        <v>0.16883116883116883</v>
+      </c>
+      <c r="F26" s="20">
+        <f t="shared" ref="F26:I26" si="8">F6/F$12</f>
+        <v>0.20860927152317882</v>
+      </c>
+      <c r="G26" s="20">
+        <f t="shared" si="8"/>
+        <v>0.16810344827586207</v>
+      </c>
+      <c r="H26" s="20">
+        <f t="shared" si="8"/>
+        <v>0.2</v>
+      </c>
+      <c r="I26" s="20">
+        <f t="shared" si="8"/>
+        <v>0.17391304347826086</v>
+      </c>
+      <c r="J26" s="20">
+        <f t="shared" ref="J26" si="9">J6/J$12</f>
+        <v>0.18595041322314049</v>
+      </c>
+      <c r="L26" s="15">
+        <v>8</v>
+      </c>
+      <c r="M26" s="16">
+        <v>26</v>
+      </c>
+      <c r="N26" s="16">
+        <v>63</v>
+      </c>
+      <c r="O26" s="16">
+        <v>39</v>
+      </c>
+      <c r="P26" s="16">
+        <v>3</v>
+      </c>
+      <c r="Q26" s="16">
+        <v>4</v>
+      </c>
+      <c r="R26" s="17">
+        <f>SUM(M26:Q26)</f>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="27" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D27" s="15">
+        <v>9</v>
+      </c>
+      <c r="E27" s="20">
+        <f t="shared" ref="E27:I31" si="10">E7/E$12</f>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="F27" s="20">
+        <f t="shared" si="10"/>
+        <v>0.18211920529801323</v>
+      </c>
+      <c r="G27" s="20">
+        <f t="shared" si="10"/>
+        <v>0.14655172413793102</v>
+      </c>
+      <c r="H27" s="20">
+        <f t="shared" si="10"/>
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="I27" s="20">
+        <f t="shared" si="10"/>
+        <v>0.17391304347826086</v>
+      </c>
+      <c r="J27" s="20">
+        <f t="shared" ref="J27" si="11">J7/J$12</f>
+        <v>0.16115702479338842</v>
+      </c>
+      <c r="L27" s="15">
+        <v>9</v>
+      </c>
+      <c r="M27" s="16">
+        <v>22</v>
+      </c>
+      <c r="N27" s="16">
+        <v>55</v>
+      </c>
+      <c r="O27" s="16">
+        <v>34</v>
+      </c>
+      <c r="P27" s="16">
+        <v>2</v>
+      </c>
+      <c r="Q27" s="16">
+        <v>4</v>
+      </c>
+      <c r="R27" s="17">
+        <f t="shared" ref="R27:R31" si="12">SUM(M27:Q27)</f>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="28" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D28" s="15">
+        <v>10</v>
+      </c>
+      <c r="E28" s="20">
+        <f t="shared" si="10"/>
+        <v>0.19480519480519481</v>
+      </c>
+      <c r="F28" s="20">
+        <f t="shared" si="10"/>
+        <v>0.17549668874172186</v>
+      </c>
+      <c r="G28" s="20">
+        <f t="shared" si="10"/>
+        <v>0.15948275862068967</v>
+      </c>
+      <c r="H28" s="20">
+        <f t="shared" si="10"/>
+        <v>0.2</v>
+      </c>
+      <c r="I28" s="20">
+        <f t="shared" si="10"/>
+        <v>0.17391304347826086</v>
+      </c>
+      <c r="J28" s="20">
+        <f t="shared" ref="J28" si="13">J8/J$12</f>
+        <v>0.17493112947658401</v>
+      </c>
+      <c r="L28" s="15">
+        <v>10</v>
+      </c>
+      <c r="M28" s="16">
+        <v>30</v>
+      </c>
+      <c r="N28" s="16">
+        <v>53</v>
+      </c>
+      <c r="O28" s="16">
+        <v>37</v>
+      </c>
+      <c r="P28" s="16">
+        <v>3</v>
+      </c>
+      <c r="Q28" s="16">
+        <v>4</v>
+      </c>
+      <c r="R28" s="17">
+        <f t="shared" si="12"/>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="29" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D29" s="15">
+        <v>11</v>
+      </c>
+      <c r="E29" s="20">
+        <f t="shared" si="10"/>
+        <v>0.16233766233766234</v>
+      </c>
+      <c r="F29" s="20">
+        <f t="shared" si="10"/>
+        <v>0.13576158940397351</v>
+      </c>
+      <c r="G29" s="20">
+        <f t="shared" si="10"/>
+        <v>0.20258620689655171</v>
+      </c>
+      <c r="H29" s="20">
+        <f t="shared" si="10"/>
+        <v>0.2</v>
+      </c>
+      <c r="I29" s="20">
+        <f t="shared" si="10"/>
+        <v>0.17391304347826086</v>
+      </c>
+      <c r="J29" s="20">
+        <f t="shared" ref="J29" si="14">J9/J$12</f>
+        <v>0.16528925619834711</v>
+      </c>
+      <c r="L29" s="15">
+        <v>11</v>
+      </c>
+      <c r="M29" s="16">
+        <v>25</v>
+      </c>
+      <c r="N29" s="16">
+        <v>41</v>
+      </c>
+      <c r="O29" s="16">
+        <v>47</v>
+      </c>
+      <c r="P29" s="16">
+        <v>3</v>
+      </c>
+      <c r="Q29" s="16">
+        <v>4</v>
+      </c>
+      <c r="R29" s="17">
+        <f t="shared" si="12"/>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="30" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D30" s="15">
+        <v>12</v>
+      </c>
+      <c r="E30" s="20">
+        <f t="shared" si="10"/>
+        <v>0.19480519480519481</v>
+      </c>
+      <c r="F30" s="20">
+        <f t="shared" si="10"/>
+        <v>0.16556291390728478</v>
+      </c>
+      <c r="G30" s="20">
+        <f t="shared" si="10"/>
+        <v>0.15948275862068967</v>
+      </c>
+      <c r="H30" s="20">
+        <f t="shared" si="10"/>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="I30" s="20">
+        <f t="shared" si="10"/>
+        <v>0.17391304347826086</v>
+      </c>
+      <c r="J30" s="20">
+        <f t="shared" ref="J30" si="15">J10/J$12</f>
+        <v>0.16804407713498623</v>
+      </c>
+      <c r="L30" s="15">
+        <v>12</v>
+      </c>
+      <c r="M30" s="16">
+        <v>30</v>
+      </c>
+      <c r="N30" s="16">
+        <v>50</v>
+      </c>
+      <c r="O30" s="16">
+        <v>37</v>
+      </c>
+      <c r="P30" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q30" s="16">
+        <v>4</v>
+      </c>
+      <c r="R30" s="17">
+        <f t="shared" si="12"/>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="31" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D31" s="15">
+        <v>13</v>
+      </c>
+      <c r="E31" s="20">
+        <f t="shared" si="10"/>
+        <v>0.13636363636363635</v>
+      </c>
+      <c r="F31" s="20">
+        <f t="shared" si="10"/>
+        <v>0.13245033112582782</v>
+      </c>
+      <c r="G31" s="20">
+        <f t="shared" si="10"/>
+        <v>0.16379310344827586</v>
+      </c>
+      <c r="H31" s="20">
+        <f t="shared" si="10"/>
+        <v>0.2</v>
+      </c>
+      <c r="I31" s="20">
+        <f t="shared" si="10"/>
+        <v>0.13043478260869565</v>
+      </c>
+      <c r="J31" s="20">
+        <f t="shared" ref="J31" si="16">J11/J$12</f>
+        <v>0.14462809917355371</v>
+      </c>
+      <c r="L31" s="15">
+        <v>13</v>
+      </c>
+      <c r="M31" s="16">
+        <v>21</v>
+      </c>
+      <c r="N31" s="16">
+        <v>40</v>
+      </c>
+      <c r="O31" s="16">
+        <v>38</v>
+      </c>
+      <c r="P31" s="16">
+        <v>3</v>
+      </c>
+      <c r="Q31" s="16">
+        <v>3</v>
+      </c>
+      <c r="R31" s="17">
+        <f t="shared" si="12"/>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="32" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D32" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" s="21">
+        <f>E12/$J12</f>
+        <v>0.21212121212121213</v>
+      </c>
+      <c r="F32" s="21">
+        <f t="shared" ref="F32:J32" si="17">F12/$J12</f>
+        <v>0.41597796143250687</v>
+      </c>
+      <c r="G32" s="21">
+        <f t="shared" si="17"/>
+        <v>0.31955922865013775</v>
+      </c>
+      <c r="H32" s="21">
+        <f t="shared" si="17"/>
+        <v>2.0661157024793389E-2</v>
+      </c>
+      <c r="I32" s="21">
+        <f t="shared" si="17"/>
+        <v>3.1680440771349863E-2</v>
+      </c>
+      <c r="J32" s="21">
+        <f t="shared" si="17"/>
+        <v>1</v>
+      </c>
+      <c r="L32" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="M32" s="19">
+        <f>SUM(M26:M31)</f>
+        <v>154</v>
+      </c>
+      <c r="N32" s="19">
+        <f>SUM(N26:N31)</f>
+        <v>302</v>
+      </c>
+      <c r="O32" s="19">
+        <f>SUM(O26:O31)</f>
+        <v>232</v>
+      </c>
+      <c r="P32" s="19">
+        <f>SUM(P26:P31)</f>
+        <v>15</v>
+      </c>
+      <c r="Q32" s="19">
+        <f>SUM(Q26:Q31)</f>
+        <v>23</v>
+      </c>
+      <c r="R32" s="19">
+        <f>SUM(R26:R31)</f>
+        <v>726</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="D4:J4"/>
+    <mergeCell ref="L4:R4"/>
+    <mergeCell ref="D14:J14"/>
+    <mergeCell ref="L14:R14"/>
+    <mergeCell ref="D24:J24"/>
+    <mergeCell ref="L24:R24"/>
+  </mergeCells>
+  <conditionalFormatting sqref="E26:E31">
+    <cfRule type="dataBar" priority="7">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF008AEF"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{42E3ED88-B5A8-4039-A4DC-A62EFB662788}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F26:F31">
+    <cfRule type="dataBar" priority="6">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF008AEF"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{C4699132-632D-4CDE-A95D-5714483308EB}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E32:I32">
+    <cfRule type="dataBar" priority="5">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{5C3F2227-055C-4D67-B456-27FE0A798F09}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G26:G31">
+    <cfRule type="dataBar" priority="4">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF008AEF"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{9D9B813A-B24D-45CC-AB4F-78F3FECD7595}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H26:H31">
+    <cfRule type="dataBar" priority="3">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF008AEF"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{7572D534-0AD6-4838-8213-4B538710C491}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I26:J31">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF008AEF"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{074DBB52-E767-4541-9135-2FE530525398}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M26:N31">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF008AEF"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{AEE8D100-B094-418F-8FB7-3ACF30B1303D}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{42E3ED88-B5A8-4039-A4DC-A62EFB662788}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF008AEF"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E26:E31</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{C4699132-632D-4CDE-A95D-5714483308EB}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF008AEF"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F26:F31</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{5C3F2227-055C-4D67-B456-27FE0A798F09}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E32:I32</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{9D9B813A-B24D-45CC-AB4F-78F3FECD7595}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF008AEF"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>G26:G31</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{7572D534-0AD6-4838-8213-4B538710C491}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF008AEF"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H26:H31</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{074DBB52-E767-4541-9135-2FE530525398}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF008AEF"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>I26:J31</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{AEE8D100-B094-418F-8FB7-3ACF30B1303D}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF008AEF"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>M26:N31</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>